<commit_message>
added solidworks and LRA motor reference
</commit_message>
<xml_diff>
--- a/Datasheets/Specs of components.xlsx
+++ b/Datasheets/Specs of components.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B1D98D-CB43-4755-AA28-E574DB3B09EA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D75558-E86F-428B-AE5C-26F7F1A27A2D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>vpm2 Motor</t>
   </si>
@@ -58,12 +58,6 @@
     <t>3 V (2.5 - 3.5)</t>
   </si>
   <si>
-    <t>32 +- 20%</t>
-  </si>
-  <si>
-    <t>6 +- 5%</t>
-  </si>
-  <si>
     <t xml:space="preserve"> G0832012 LRA</t>
   </si>
   <si>
@@ -77,6 +71,15 @@
   </si>
   <si>
     <t>235 Hz</t>
+  </si>
+  <si>
+    <t>32 +- 20% Ohm</t>
+  </si>
+  <si>
+    <t>6 +- 5% Ohm</t>
+  </si>
+  <si>
+    <t>22 +- 18% Ohm</t>
   </si>
 </sst>
 </file>
@@ -445,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,7 +462,7 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -473,7 +476,7 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -495,10 +498,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -517,16 +523,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>